<commit_message>
changed mapping of SNAQ[x] profiles
</commit_message>
<xml_diff>
--- a/Mappings/SNAQ65+Score - STU3.xlsx
+++ b/Mappings/SNAQ65+Score - STU3.xlsx
@@ -10,19 +10,20 @@
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Metadata" sheetId="2" r:id="rId2"/>
     <sheet name="Information Model" sheetId="3" r:id="rId3"/>
-    <sheet name="Data" sheetId="4" r:id="rId4"/>
-    <sheet name="SNAQ65+AppetiteScoreCodelist" sheetId="5" r:id="rId5"/>
-    <sheet name="SNAQ65+ExerciseScoreCodelist" sheetId="6" r:id="rId6"/>
-    <sheet name="SNAQ65+UpperarmCircumferenceCod" sheetId="7" r:id="rId7"/>
-    <sheet name="SNAQ65+WeightLossScoreCodelist" sheetId="8" r:id="rId8"/>
-    <sheet name="Terms of Use" sheetId="9" r:id="rId9"/>
+    <sheet name="Sheet1" sheetId="10" r:id="rId4"/>
+    <sheet name="Data" sheetId="4" r:id="rId5"/>
+    <sheet name="SNAQ65+AppetiteScoreCodelist" sheetId="5" r:id="rId6"/>
+    <sheet name="SNAQ65+ExerciseScoreCodelist" sheetId="6" r:id="rId7"/>
+    <sheet name="SNAQ65+UpperarmCircumferenceCod" sheetId="7" r:id="rId8"/>
+    <sheet name="SNAQ65+WeightLossScoreCodelist" sheetId="8" r:id="rId9"/>
+    <sheet name="Terms of Use" sheetId="9" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="196">
   <si>
     <t>Subject</t>
   </si>
@@ -528,9 +529,6 @@
     <t>Maps to</t>
   </si>
   <si>
-    <t>Observation</t>
-  </si>
-  <si>
     <t>Observation.valueQuantity</t>
   </si>
   <si>
@@ -555,18 +553,81 @@
     <t>Observation.component.exerciseScore.valueCodeableConcept</t>
   </si>
   <si>
-    <t>Waardebereik: 0-5
+    <t>If one of the component Scores is present, other scores (other than TotalScore) are required</t>
+  </si>
+  <si>
+    <t>Equivalence</t>
+  </si>
+  <si>
+    <t>nl-core-observation</t>
+  </si>
+  <si>
+    <t>equal</t>
+  </si>
+  <si>
+    <t>Valueset mapping</t>
+  </si>
+  <si>
+    <t>No SNOMED code available. Check BITS issue ZIB-287 for progress</t>
+  </si>
+  <si>
+    <t>ValueRange: 0-5
 If  component scores are not present, then Total score is Required.</t>
   </si>
   <si>
-    <t>If one of the component Scores is present, other scores (other than TotalScore) are required</t>
+    <t>Checkbox searched for existing profiles / implementation on:</t>
+  </si>
+  <si>
+    <t>Checkbox!</t>
+  </si>
+  <si>
+    <t>Searchwords</t>
+  </si>
+  <si>
+    <t>Found results:</t>
+  </si>
+  <si>
+    <t>HL7 FHIR Specification</t>
+  </si>
+  <si>
+    <t>HL7 FHIR profiles</t>
+  </si>
+  <si>
+    <t>no relevant</t>
+  </si>
+  <si>
+    <t>HL7 FHIR profiles - latest version latest version (build)</t>
+  </si>
+  <si>
+    <t>HL7 FHIR extension registry</t>
+  </si>
+  <si>
+    <t>HL7 FHIR extension registry - latest version (build)</t>
+  </si>
+  <si>
+    <t>HL7 FHIR implementation guides (e.g. Argonaut)</t>
+  </si>
+  <si>
+    <t>Simplifier.net</t>
+  </si>
+  <si>
+    <t>Zulip (chat.fhir.org)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Google </t>
+  </si>
+  <si>
+    <t>SNAQ65+Score, SNAQ65+, Malnutrion</t>
+  </si>
+  <si>
+    <t>SNAQ65+Score, SNAQ65+ Malnutrion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
@@ -603,8 +664,20 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -624,6 +697,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD3D3D3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -688,10 +766,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -742,8 +821,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -754,6 +844,166 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp17.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp26.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp27.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp28.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp29.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp30.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp31.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp32.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp33.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp34.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp35.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp36.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp37.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp38.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp39.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp40.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -863,6 +1113,1571 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4097" name="Check Box 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4097"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4098" name="Check Box 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4098"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4099" name="Check Box 3" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4099"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4100" name="Check Box 4" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4100"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4101" name="Check Box 5" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4101"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4102" name="Check Box 6" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4102"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4103" name="Check Box 7" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4103"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4104" name="Check Box 8" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4104"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4105" name="Check Box 9" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4105"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4106" name="Check Box 10" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4106"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4107" name="Check Box 11" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4107"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4108" name="Check Box 12" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4108"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4109" name="Check Box 13" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4109"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4110" name="Check Box 14" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4110"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4111" name="Check Box 15" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4111"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4112" name="Check Box 16" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4112"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4113" name="Check Box 17" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4113"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4114" name="Check Box 18" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4114"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4115" name="Check Box 19" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4115"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4116" name="Check Box 20" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4116"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4117" name="Check Box 21" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4117"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4118" name="Check Box 22" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4118"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4119" name="Check Box 23" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4119"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4120" name="Check Box 24" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4120"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="704850" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4121" name="Check Box 25" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4121"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="704850" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4122" name="Check Box 26" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4122"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="704850" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4123" name="Check Box 27" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4123"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="704850" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4124" name="Check Box 28" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4124"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="704850" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4125" name="Check Box 29" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4125"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="704850" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4126" name="Check Box 30" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4126"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="704850" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4127" name="Check Box 31" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4127"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="704850" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4128" name="Check Box 32" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4128"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="704850" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4129" name="Check Box 33" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4129"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="704850" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4130" name="Check Box 34" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4130"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="704850" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4131" name="Check Box 35" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4131"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="704850" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4132" name="Check Box 36" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4132"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="704850" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4133" name="Check Box 37" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4133"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="704850" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4134" name="Check Box 38" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4134"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="704850" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4135" name="Check Box 39" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4135"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="704850" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4136" name="Check Box 40" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4136"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -1287,6 +3102,52 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="2" max="2" width="150" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2">
+      <c r="B2" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" ht="140.25">
+      <c r="B3" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" ht="25.5">
+      <c r="B5" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
+      <c r="B6" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" ht="38.25">
+      <c r="B7" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C25"/>
@@ -1300,10 +3161,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="17"/>
+      <c r="C2" s="18"/>
     </row>
     <row r="3" spans="2:3">
       <c r="B3" s="2" t="s">
@@ -1510,11 +3371,1001 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="50" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="F2" s="23"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="22" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="22" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="22" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="22" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="22" t="s">
+        <v>191</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="22" t="s">
+        <v>192</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="22" t="s">
+        <v>193</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>186</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4097" r:id="rId3" name="Check Box 1">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4098" r:id="rId4" name="Check Box 2">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4099" r:id="rId5" name="Check Box 3">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>1</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4100" r:id="rId6" name="Check Box 4">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4101" r:id="rId7" name="Check Box 5">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4102" r:id="rId8" name="Check Box 6">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4103" r:id="rId9" name="Check Box 7">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4104" r:id="rId10" name="Check Box 8">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4105" r:id="rId11" name="Check Box 9">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4106" r:id="rId12" name="Check Box 10">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4107" r:id="rId13" name="Check Box 11">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4108" r:id="rId14" name="Check Box 12">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4109" r:id="rId15" name="Check Box 13">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4110" r:id="rId16" name="Check Box 14">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4111" r:id="rId17" name="Check Box 15">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4112" r:id="rId18" name="Check Box 16">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4113" r:id="rId19" name="Check Box 17">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4114" r:id="rId20" name="Check Box 18">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4115" r:id="rId21" name="Check Box 19">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4116" r:id="rId22" name="Check Box 20">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4117" r:id="rId23" name="Check Box 21">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4118" r:id="rId24" name="Check Box 22">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4119" r:id="rId25" name="Check Box 23">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4120" r:id="rId26" name="Check Box 24">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4121" r:id="rId27" name="Check Box 25">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4122" r:id="rId28" name="Check Box 26">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4123" r:id="rId29" name="Check Box 27">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4124" r:id="rId30" name="Check Box 28">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4125" r:id="rId31" name="Check Box 29">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4126" r:id="rId32" name="Check Box 30">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4127" r:id="rId33" name="Check Box 31">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4128" r:id="rId34" name="Check Box 32">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4129" r:id="rId35" name="Check Box 33">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4130" r:id="rId36" name="Check Box 34">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4131" r:id="rId37" name="Check Box 35">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4132" r:id="rId38" name="Check Box 36">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4133" r:id="rId39" name="Check Box 37">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4134" r:id="rId40" name="Check Box 38">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4135" r:id="rId41" name="Check Box 39">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4136" r:id="rId42" name="Check Box 40">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>142875</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:R10"/>
+  <dimension ref="B2:T10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1529,11 +4380,12 @@
     <col min="14" max="14" width="20" customWidth="1"/>
     <col min="15" max="15" width="30" customWidth="1"/>
     <col min="16" max="16" width="59.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="30" customWidth="1"/>
-    <col min="18" max="18" width="20" customWidth="1"/>
+    <col min="17" max="18" width="59.28515625" customWidth="1"/>
+    <col min="19" max="19" width="30" customWidth="1"/>
+    <col min="20" max="20" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18">
+    <row r="2" spans="2:20">
       <c r="B2" s="5" t="s">
         <v>53</v>
       </c>
@@ -1569,14 +4421,20 @@
       <c r="P2" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="R2" s="1" t="s">
+      <c r="Q2" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="R2" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="2:18" ht="25.5">
+    <row r="3" spans="2:20" ht="25.5">
       <c r="B3" s="8" t="s">
         <v>70</v>
       </c>
@@ -1602,12 +4460,16 @@
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
       <c r="P3" s="4" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
-    </row>
-    <row r="4" spans="2:18" ht="63.75">
+      <c r="S3" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="T3" s="4"/>
+    </row>
+    <row r="4" spans="2:20" ht="63.75">
       <c r="B4" s="11"/>
       <c r="C4" s="12" t="s">
         <v>75</v>
@@ -1639,14 +4501,20 @@
         <v>82</v>
       </c>
       <c r="P4" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" spans="2:18" ht="25.5">
+        <v>169</v>
+      </c>
+      <c r="Q4" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="R4" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="S4" s="15"/>
+      <c r="T4" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20" ht="25.5">
       <c r="B5" s="11"/>
       <c r="C5" s="12" t="s">
         <v>83</v>
@@ -1678,12 +4546,18 @@
         <v>87</v>
       </c>
       <c r="P5" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="2"/>
-    </row>
-    <row r="6" spans="2:18">
+        <v>170</v>
+      </c>
+      <c r="Q5" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="R5" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="S5" s="15"/>
+      <c r="T5" s="2"/>
+    </row>
+    <row r="6" spans="2:20">
       <c r="B6" s="11"/>
       <c r="C6" s="12" t="s">
         <v>88</v>
@@ -1715,12 +4589,18 @@
         <v>92</v>
       </c>
       <c r="P6" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="2"/>
-    </row>
-    <row r="7" spans="2:18" ht="25.5">
+        <v>171</v>
+      </c>
+      <c r="Q6" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="R6" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="S6" s="15"/>
+      <c r="T6" s="2"/>
+    </row>
+    <row r="7" spans="2:20" ht="25.5">
       <c r="B7" s="11"/>
       <c r="C7" s="12" t="s">
         <v>93</v>
@@ -1752,12 +4632,18 @@
         <v>97</v>
       </c>
       <c r="P7" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="2"/>
-    </row>
-    <row r="8" spans="2:18" ht="76.5">
+        <v>172</v>
+      </c>
+      <c r="Q7" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="R7" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="S7" s="15"/>
+      <c r="T7" s="2"/>
+    </row>
+    <row r="8" spans="2:20" ht="76.5">
       <c r="B8" s="11"/>
       <c r="C8" s="12" t="s">
         <v>98</v>
@@ -1787,14 +4673,18 @@
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
       <c r="P8" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="9" spans="2:18">
+        <v>165</v>
+      </c>
+      <c r="Q8" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="R8" s="16"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="16" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20">
       <c r="B9" s="11"/>
       <c r="C9" s="12" t="s">
         <v>103</v>
@@ -1824,12 +4714,16 @@
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
       <c r="P9" s="16" t="s">
-        <v>167</v>
-      </c>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-    </row>
-    <row r="10" spans="2:18" ht="25.5">
+        <v>166</v>
+      </c>
+      <c r="Q9" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="R9" s="16"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+    </row>
+    <row r="10" spans="2:20" ht="25.5">
       <c r="B10" s="11"/>
       <c r="C10" s="12" t="s">
         <v>109</v>
@@ -1861,10 +4755,14 @@
       </c>
       <c r="O10" s="2"/>
       <c r="P10" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
+        <v>167</v>
+      </c>
+      <c r="Q10" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="R10" s="16"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1876,105 +4774,6 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="J3:J9" numberStoredAsText="1"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:H6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="28" customWidth="1"/>
-    <col min="8" max="8" width="32" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="3:8">
-      <c r="C3" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-    </row>
-    <row r="4" spans="3:8">
-      <c r="C4" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="3:8" ht="25.5">
-      <c r="C5" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="6" spans="3:8" ht="25.5">
-      <c r="C6" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:H3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="D5:E6" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1995,16 +4794,16 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:8">
-      <c r="C3" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
+      <c r="C3" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="3:8">
       <c r="C4" s="14" t="s">
@@ -2028,42 +4827,42 @@
     </row>
     <row r="5" spans="3:8" ht="25.5">
       <c r="C5" s="2" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>123</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="3:8" ht="25.5">
       <c r="C6" s="2" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>106</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2094,16 +4893,16 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:8">
-      <c r="C3" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
+      <c r="C3" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="3:8">
       <c r="C4" s="14" t="s">
@@ -2127,42 +4926,42 @@
     </row>
     <row r="5" spans="3:8" ht="25.5">
       <c r="C5" s="2" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>123</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="3:8" ht="25.5">
       <c r="C6" s="2" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>147</v>
+        <v>106</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2193,16 +4992,16 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:8">
-      <c r="C3" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
+      <c r="C3" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="3:8">
       <c r="C4" s="14" t="s">
@@ -2226,42 +5025,42 @@
     </row>
     <row r="5" spans="3:8" ht="25.5">
       <c r="C5" s="2" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>123</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="3:8" ht="25.5">
       <c r="C6" s="2" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>147</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -2278,47 +5077,100 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B7"/>
+  <dimension ref="C3:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="2" max="2" width="150" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="4" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="21" customWidth="1"/>
+    <col min="7" max="7" width="28" customWidth="1"/>
+    <col min="8" max="8" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2">
-      <c r="B2" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" ht="140.25">
-      <c r="B3" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2">
-      <c r="B4" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" ht="25.5">
-      <c r="B5" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2">
-      <c r="B6" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" ht="38.25">
-      <c r="B7" s="2" t="s">
-        <v>163</v>
+    <row r="3" spans="3:8">
+      <c r="C3" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+    </row>
+    <row r="4" spans="3:8">
+      <c r="C4" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" ht="25.5">
+      <c r="C5" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" ht="25.5">
+      <c r="C6" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:H3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="D5:E6" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -2514,18 +5366,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2548,18 +5400,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6650378-71B4-4844-BD0B-6D189D289655}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{215A4730-503F-40B0-8373-5D2A809E2679}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6650378-71B4-4844-BD0B-6D189D289655}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Check and cosmetic changes to SNAQ*/StrongKids score zibs
</commit_message>
<xml_diff>
--- a/Mappings/SNAQ65+Score - STU3.xlsx
+++ b/Mappings/SNAQ65+Score - STU3.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edelman\Nictiz-STU3-Zib2017\Mappings\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D093782-EC6F-4ADA-95B7-F9BE24AAC73A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="630" windowWidth="27495" windowHeight="13995" activeTab="3"/>
+    <workbookView xWindow="630" yWindow="630" windowWidth="27495" windowHeight="13995" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Metadata" sheetId="2" r:id="rId2"/>
     <sheet name="Information Model" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="10" r:id="rId4"/>
+    <sheet name="Research" sheetId="10" r:id="rId4"/>
     <sheet name="Data" sheetId="4" r:id="rId5"/>
     <sheet name="SNAQ65+AppetiteScoreCodelist" sheetId="5" r:id="rId6"/>
     <sheet name="SNAQ65+ExerciseScoreCodelist" sheetId="6" r:id="rId7"/>
@@ -626,8 +632,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
@@ -821,9 +827,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -831,6 +834,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -841,6 +847,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1018,7 +1027,13 @@
     <xdr:ext cx="2856900" cy="618995"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1025" name="Picture 1"/>
+        <xdr:cNvPr id="1025" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1053,7 +1068,13 @@
     <xdr:ext cx="1428750" cy="504825"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1026" name="Picture 2"/>
+        <xdr:cNvPr id="1026" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1088,7 +1109,13 @@
     <xdr:ext cx="10325100" cy="5324475"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1025" name="Picture 1"/>
+        <xdr:cNvPr id="1025" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000001040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1140,11 +1167,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4097"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000001100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1152,6 +1182,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1181,11 +1234,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4098"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1193,6 +1249,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1222,11 +1301,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4099"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1234,6 +1316,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1263,11 +1368,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4100"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1275,6 +1383,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1304,11 +1435,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4101"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1316,6 +1450,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1345,11 +1502,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4102"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000006100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1357,6 +1517,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1386,11 +1569,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4103"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1398,6 +1584,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1427,11 +1636,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4104"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000008100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1439,6 +1651,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1468,11 +1703,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4105"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000009100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1480,6 +1718,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1509,11 +1770,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4106"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000A100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1521,6 +1785,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1550,11 +1837,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4107"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000B100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1562,6 +1852,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1591,11 +1904,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4108"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000C100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1603,6 +1919,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1632,11 +1971,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4109"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000D100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1644,6 +1986,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1673,11 +2038,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4110"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000E100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1685,6 +2053,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1714,11 +2105,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4111"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000F100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1726,6 +2120,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1755,11 +2172,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4112"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000010100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1767,6 +2187,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1796,11 +2239,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4113"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000011100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1808,6 +2254,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1837,11 +2306,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4114"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000012100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1849,6 +2321,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1878,11 +2373,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4115"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000013100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1890,6 +2388,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1919,11 +2440,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4116"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000014100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1931,6 +2455,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1960,11 +2507,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4117"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000015100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1972,6 +2522,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2001,11 +2574,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4118"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000016100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2013,6 +2589,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2042,11 +2641,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4119"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000017100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2054,6 +2656,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2083,11 +2708,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4120"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000018100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2095,6 +2723,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2104,14 +2755,19 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="704850" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4121" name="Check Box 25" hidden="1">
@@ -2119,11 +2775,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4121"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000019100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2131,23 +2790,51 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="704850" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4122" name="Check Box 26" hidden="1">
@@ -2155,11 +2842,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4122"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001A100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2167,23 +2857,51 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="704850" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4123" name="Check Box 27" hidden="1">
@@ -2191,11 +2909,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4123"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001B100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2203,23 +2924,51 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="704850" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4124" name="Check Box 28" hidden="1">
@@ -2227,11 +2976,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4124"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001C100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2239,23 +2991,51 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="704850" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4125" name="Check Box 29" hidden="1">
@@ -2263,11 +3043,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4125"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001D100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2275,23 +3058,51 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="704850" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4126" name="Check Box 30" hidden="1">
@@ -2299,11 +3110,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4126"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001E100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2311,23 +3125,51 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="704850" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4127" name="Check Box 31" hidden="1">
@@ -2335,11 +3177,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4127"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001F100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2347,23 +3192,51 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="704850" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4128" name="Check Box 32" hidden="1">
@@ -2371,11 +3244,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4128"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000020100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2383,23 +3259,51 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="704850" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4129" name="Check Box 33" hidden="1">
@@ -2407,11 +3311,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4129"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000021100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2419,23 +3326,51 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="704850" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4130" name="Check Box 34" hidden="1">
@@ -2443,11 +3378,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4130"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000022100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2455,23 +3393,51 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="704850" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4131" name="Check Box 35" hidden="1">
@@ -2479,11 +3445,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4131"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000023100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2491,23 +3460,51 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="704850" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4132" name="Check Box 36" hidden="1">
@@ -2515,11 +3512,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4132"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000024100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2527,23 +3527,51 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="704850" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4133" name="Check Box 37" hidden="1">
@@ -2551,11 +3579,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4133"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000025100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2563,23 +3594,51 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="704850" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4134" name="Check Box 38" hidden="1">
@@ -2587,11 +3646,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4134"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000026100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2599,23 +3661,51 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="704850" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4135" name="Check Box 39" hidden="1">
@@ -2623,11 +3713,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4135"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000027100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2635,23 +3728,51 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="704850" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4136" name="Check Box 40" hidden="1">
@@ -2659,11 +3780,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4136"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000028100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2671,10 +3795,33 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -2724,7 +3871,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2757,9 +3904,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2792,6 +3956,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2967,18 +4148,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2986,7 +4167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -2994,7 +4175,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -3002,7 +4183,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
@@ -3010,7 +4191,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -3018,7 +4199,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
@@ -3026,7 +4207,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
@@ -3034,7 +4215,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
@@ -3042,7 +4223,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
@@ -3050,7 +4231,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
@@ -3058,7 +4239,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="89.25">
+    <row r="12" spans="2:3" ht="89.25" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>53</v>
       </c>
@@ -3066,7 +4247,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="25.5">
+    <row r="13" spans="2:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>55</v>
       </c>
@@ -3074,7 +4255,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="89.25">
+    <row r="14" spans="2:3" ht="89.25" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>57</v>
       </c>
@@ -3082,7 +4263,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="2:3" ht="25.5">
+    <row r="15" spans="2:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>59</v>
       </c>
@@ -3092,7 +4273,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1"/>
+    <hyperlink ref="C11" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -3103,42 +4284,42 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="B2:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="150" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="3" spans="2:2" ht="140.25">
+    <row r="3" spans="2:2" ht="140.25" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="4" spans="2:2">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="25.5">
+    <row r="5" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="2:2">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="38.25">
+    <row r="7" spans="2:2" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>163</v>
       </c>
@@ -3149,24 +4330,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="35" customWidth="1"/>
     <col min="3" max="3" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
-      <c r="B2" s="18" t="s">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="18"/>
-    </row>
-    <row r="3" spans="2:3">
+      <c r="C2" s="23"/>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
@@ -3174,7 +4355,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
@@ -3182,7 +4363,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
@@ -3190,7 +4371,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>26</v>
       </c>
@@ -3198,7 +4379,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
@@ -3206,7 +4387,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>28</v>
       </c>
@@ -3214,13 +4395,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="2:3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>31</v>
       </c>
@@ -3228,13 +4409,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="2:3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="2:3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
@@ -3242,13 +4423,13 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="2:3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="2:3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>37</v>
       </c>
@@ -3256,7 +4437,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="2:3">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>39</v>
       </c>
@@ -3264,7 +4445,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="2:3">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>41</v>
       </c>
@@ -3272,7 +4453,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>42</v>
       </c>
@@ -3280,7 +4461,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>43</v>
       </c>
@@ -3288,7 +4469,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>44</v>
       </c>
@@ -3296,7 +4477,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
         <v>45</v>
       </c>
@@ -3304,7 +4485,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="2:3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
         <v>46</v>
       </c>
@@ -3312,7 +4493,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="2:3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
         <v>48</v>
       </c>
@@ -3320,13 +4501,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="2:3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
         <v>50</v>
       </c>
@@ -3334,7 +4515,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
         <v>51</v>
       </c>
@@ -3354,14 +4535,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
     </row>
   </sheetData>
@@ -3371,99 +4552,99 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="50" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21" t="s">
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="22" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="F2" s="23"/>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="22" t="s">
+      <c r="F2" s="22"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="21" t="s">
         <v>185</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="21" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="22" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="22" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="21" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="22" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="21" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="22" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="21" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="22" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="21" t="s">
         <v>191</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="21" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="22" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="21" t="s">
         <v>192</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="21" t="s">
         <v>195</v>
       </c>
-      <c r="F9" s="22" t="s">
+      <c r="F9" s="21" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="22" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="21" t="s">
         <v>195</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="F10" s="21" t="s">
         <v>186</v>
       </c>
     </row>
@@ -4361,14 +5542,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:T10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="6" width="2" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
@@ -4385,7 +5566,7 @@
     <col min="20" max="20" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:20">
+    <row r="2" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
         <v>53</v>
       </c>
@@ -4434,7 +5615,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="2:20" ht="25.5">
+    <row r="3" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B3" s="8" t="s">
         <v>70</v>
       </c>
@@ -4464,12 +5645,12 @@
       </c>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
-      <c r="S3" s="20" t="s">
+      <c r="S3" s="19" t="s">
         <v>178</v>
       </c>
       <c r="T3" s="4"/>
     </row>
-    <row r="4" spans="2:20" ht="63.75">
+    <row r="4" spans="2:20" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B4" s="11"/>
       <c r="C4" s="12" t="s">
         <v>75</v>
@@ -4503,10 +5684,10 @@
       <c r="P4" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="Q4" s="19" t="s">
+      <c r="Q4" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="R4" s="19" t="s">
+      <c r="R4" s="18" t="s">
         <v>2</v>
       </c>
       <c r="S4" s="15"/>
@@ -4514,7 +5695,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="5" spans="2:20" ht="25.5">
+    <row r="5" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B5" s="11"/>
       <c r="C5" s="12" t="s">
         <v>83</v>
@@ -4548,16 +5729,16 @@
       <c r="P5" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="Q5" s="19" t="s">
+      <c r="Q5" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="R5" s="19" t="s">
+      <c r="R5" s="18" t="s">
         <v>2</v>
       </c>
       <c r="S5" s="15"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="2:20">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B6" s="11"/>
       <c r="C6" s="12" t="s">
         <v>88</v>
@@ -4591,16 +5772,16 @@
       <c r="P6" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="Q6" s="19" t="s">
+      <c r="Q6" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="R6" s="19" t="s">
+      <c r="R6" s="18" t="s">
         <v>2</v>
       </c>
       <c r="S6" s="15"/>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="2:20" ht="25.5">
+    <row r="7" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B7" s="11"/>
       <c r="C7" s="12" t="s">
         <v>93</v>
@@ -4634,16 +5815,16 @@
       <c r="P7" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="Q7" s="19" t="s">
+      <c r="Q7" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="R7" s="19" t="s">
+      <c r="R7" s="18" t="s">
         <v>2</v>
       </c>
       <c r="S7" s="15"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="2:20" ht="76.5">
+    <row r="8" spans="2:20" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B8" s="11"/>
       <c r="C8" s="12" t="s">
         <v>98</v>
@@ -4675,7 +5856,7 @@
       <c r="P8" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="Q8" s="19" t="s">
+      <c r="Q8" s="18" t="s">
         <v>176</v>
       </c>
       <c r="R8" s="16"/>
@@ -4684,7 +5865,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="9" spans="2:20">
+    <row r="9" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B9" s="11"/>
       <c r="C9" s="12" t="s">
         <v>103</v>
@@ -4716,14 +5897,14 @@
       <c r="P9" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="Q9" s="19" t="s">
+      <c r="Q9" s="18" t="s">
         <v>176</v>
       </c>
       <c r="R9" s="16"/>
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
     </row>
-    <row r="10" spans="2:20" ht="25.5">
+    <row r="10" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B10" s="11"/>
       <c r="C10" s="12" t="s">
         <v>109</v>
@@ -4757,7 +5938,7 @@
       <c r="P10" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="Q10" s="19" t="s">
+      <c r="Q10" s="18" t="s">
         <v>176</v>
       </c>
       <c r="R10" s="16"/>
@@ -4766,10 +5947,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O4" location="SNAQ65+WeightLossScoreCodelist!A1" display="SNAQ65+WeightLossScoreCodelist"/>
-    <hyperlink ref="O5" location="SNAQ65+UpperarmCircumferenceCod!A1" display="SNAQ65+UpperarmCircumferenceCodelist"/>
-    <hyperlink ref="O6" location="SNAQ65+AppetiteScoreCodelist!A1" display="SNAQ65+AppetiteScoreCodelist"/>
-    <hyperlink ref="O7" location="SNAQ65+ExerciseScoreCodelist!A1" display="SNAQ65+ExerciseScoreCodelist"/>
+    <hyperlink ref="O4" location="SNAQ65+WeightLossScoreCodelist!A1" display="SNAQ65+WeightLossScoreCodelist" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="O5" location="SNAQ65+UpperarmCircumferenceCod!A1" display="SNAQ65+UpperarmCircumferenceCodelist" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="O6" location="SNAQ65+AppetiteScoreCodelist!A1" display="SNAQ65+AppetiteScoreCodelist" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="O7" location="SNAQ65+ExerciseScoreCodelist!A1" display="SNAQ65+ExerciseScoreCodelist" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -4779,12 +5960,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="C3:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="5" width="15" customWidth="1"/>
@@ -4793,19 +5974,19 @@
     <col min="8" max="8" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:8">
-      <c r="C3" s="18" t="s">
+    <row r="3" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C3" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18" t="s">
+      <c r="D3" s="23"/>
+      <c r="E3" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-    </row>
-    <row r="4" spans="3:8">
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+    </row>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C4" s="14" t="s">
         <v>116</v>
       </c>
@@ -4825,7 +6006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:8" ht="25.5">
+    <row r="5" spans="3:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
         <v>121</v>
       </c>
@@ -4845,7 +6026,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="6" spans="3:8" ht="25.5">
+    <row r="6" spans="3:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
         <v>127</v>
       </c>
@@ -4878,12 +6059,12 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="C3:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="5" width="15" customWidth="1"/>
@@ -4892,19 +6073,19 @@
     <col min="8" max="8" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:8">
-      <c r="C3" s="18" t="s">
+    <row r="3" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C3" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18" t="s">
+      <c r="D3" s="23"/>
+      <c r="E3" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-    </row>
-    <row r="4" spans="3:8">
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+    </row>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C4" s="14" t="s">
         <v>116</v>
       </c>
@@ -4924,7 +6105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:8" ht="25.5">
+    <row r="5" spans="3:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
         <v>131</v>
       </c>
@@ -4944,7 +6125,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="3:8" ht="25.5">
+    <row r="6" spans="3:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
         <v>136</v>
       </c>
@@ -4977,12 +6158,12 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="C3:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="5" width="15" customWidth="1"/>
@@ -4991,19 +6172,19 @@
     <col min="8" max="8" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:8">
-      <c r="C3" s="18" t="s">
+    <row r="3" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C3" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18" t="s">
+      <c r="D3" s="23"/>
+      <c r="E3" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-    </row>
-    <row r="4" spans="3:8">
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+    </row>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C4" s="14" t="s">
         <v>116</v>
       </c>
@@ -5023,7 +6204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:8" ht="25.5">
+    <row r="5" spans="3:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
         <v>140</v>
       </c>
@@ -5043,7 +6224,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="6" spans="3:8" ht="25.5">
+    <row r="6" spans="3:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
         <v>145</v>
       </c>
@@ -5076,12 +6257,12 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="C3:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="5" width="15" customWidth="1"/>
@@ -5090,19 +6271,19 @@
     <col min="8" max="8" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:8">
-      <c r="C3" s="18" t="s">
+    <row r="3" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C3" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18" t="s">
+      <c r="D3" s="23"/>
+      <c r="E3" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-    </row>
-    <row r="4" spans="3:8">
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+    </row>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C4" s="14" t="s">
         <v>116</v>
       </c>
@@ -5122,7 +6303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:8" ht="25.5">
+    <row r="5" spans="3:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
         <v>150</v>
       </c>
@@ -5142,7 +6323,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="6" spans="3:8" ht="25.5">
+    <row r="6" spans="3:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
         <v>155</v>
       </c>
@@ -5175,6 +6356,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F494F4030F39954381FEDCB9F1521453" ma:contentTypeVersion="8" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="27a32a75921fafc58b02df1cc725ea53">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c9309f2a-e493-41e5-bc1f-ce1ae85ad224" xmlns:ns3="d8b013f3-f757-4442-942f-c178d59a4411" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8dd320713f27671350e0900a33d7d303" ns2:_="" ns3:_="">
     <xsd:import namespace="c9309f2a-e493-41e5-bc1f-ce1ae85ad224"/>
@@ -5365,15 +6555,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -5381,6 +6562,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6650378-71B4-4844-BD0B-6D189D289655}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{614C5B1D-DDFF-47CF-8F81-10BD2508B2D7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5399,14 +6588,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6650378-71B4-4844-BD0B-6D189D289655}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{215A4730-503F-40B0-8373-5D2A809E2679}">
   <ds:schemaRefs>

</xml_diff>